<commit_message>
Changes to Currencies in Syssettings and MINGAS1 - ELC_PRIS output is 0
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_03\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_03\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA6D102-D69E-487C-9481-31CE294844F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B3C685-9C6D-443A-B8D2-CD1BE841A750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3487,8 +3487,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="M5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>